<commit_message>
nova and warp inventory update
</commit_message>
<xml_diff>
--- a/Warp/inventory.xlsx
+++ b/Warp/inventory.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="118">
   <si>
     <t>Barracus</t>
   </si>
@@ -101,9 +101,6 @@
     <t xml:space="preserve"> Xeno Overlord</t>
   </si>
   <si>
-    <t xml:space="preserve"> Baughe</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Bane of Truth</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t xml:space="preserve"> Flank</t>
   </si>
   <si>
-    <t>Baughe(2)</t>
-  </si>
-  <si>
     <t>Halcyon</t>
   </si>
   <si>
@@ -233,15 +227,9 @@
     <t xml:space="preserve"> Cadmus</t>
   </si>
   <si>
-    <t xml:space="preserve"> Xanadu Ultra</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Tabitha</t>
   </si>
   <si>
-    <t xml:space="preserve"> The Tenacious</t>
-  </si>
-  <si>
     <t xml:space="preserve">Noble Defiance </t>
   </si>
   <si>
@@ -326,7 +314,70 @@
     <t xml:space="preserve"> valiant knight</t>
   </si>
   <si>
-    <t xml:space="preserve"> Constantine</t>
+    <t xml:space="preserve"> Inferno Demon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kylen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Galereaver</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stronghold Fortifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tikalan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ironclad Troop</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Earnest Pursuer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sacred Sanctuary</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jilted Baughe(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 Dreamweaver</t>
+  </si>
+  <si>
+    <t>Masterwork Aegis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stormreaver</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Baughe #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elite Soldier</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Xanadu Tetra</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ayrkrane Syn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Greatheart</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Serraco</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ezamit (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ascendant</t>
   </si>
 </sst>
 </file>
@@ -671,26 +722,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A49"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="22.28515625" style="1"/>
+    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="22.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -698,88 +762,103 @@
       <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -790,34 +869,78 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>5</v>
@@ -832,52 +955,58 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -885,94 +1014,105 @@
         <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -980,9 +1120,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="129" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>20</v>
@@ -991,85 +1131,79 @@
         <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="I30" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:10" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="78" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>24</v>
@@ -1078,9 +1212,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="78" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>22</v>
@@ -1089,13 +1223,13 @@
         <v>4</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>23</v>
@@ -1104,39 +1238,45 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="78" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="H37" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>22</v>
@@ -1156,29 +1296,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:10" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>22</v>
@@ -1187,69 +1327,69 @@
         <v>18</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:10" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>10</v>
@@ -1258,11 +1398,34 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:C51">

</xml_diff>